<commit_message>
Update sprint excel sheet
</commit_message>
<xml_diff>
--- a/doc/sprints.xlsx
+++ b/doc/sprints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauli\Documents\TU\repositories\SEM\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravis\projects\GitProjects\sem-repo-17a\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB20716E-58D6-4859-96B3-37B144B5BC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B73E000-8C51-4A3A-BF69-AC69398A39AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" activeTab="6" xr2:uid="{58667ADA-671B-4355-9B89-7418DDCFDFF4}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="sprint_4" sheetId="9" r:id="rId4"/>
     <sheet name="sprint_4 old" sheetId="6" r:id="rId5"/>
     <sheet name="sprint_5" sheetId="8" r:id="rId6"/>
-    <sheet name="sprint_6" sheetId="11" r:id="rId7"/>
+    <sheet name="sprint_6to9(vacation)" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="116">
   <si>
     <t>User Story #</t>
   </si>
@@ -366,17 +366,35 @@
     <t>Pauline</t>
   </si>
   <si>
-    <t>actual effort for stuff from w5</t>
-  </si>
-  <si>
-    <t>all</t>
+    <t>All</t>
+  </si>
+  <si>
+    <t>2 hour</t>
+  </si>
+  <si>
+    <t>2,5 hours</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>It revealed I missinterpreted something in a previous issue and I also had to go fix that</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +405,12 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -565,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -656,25 +680,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -849,10 +860,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}" name="Table1" displayName="Table1" ref="A1:H32" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}" name="Table1" displayName="Table1" ref="A1:H32" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:H32" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story " dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story " dataDxfId="10"/>
     <tableColumn id="8" xr3:uid="{E40A33E7-2DA6-4331-8AE0-2CAF1EE47083}" name="Issue #"/>
     <tableColumn id="2" xr3:uid="{70831594-7EAC-447C-AFB7-FEF4536D539F}" name="Task#"/>
     <tableColumn id="3" xr3:uid="{0DA9E85B-5521-4636-9DE5-1724D932B621}" name="Task assigned to"/>
@@ -866,7 +877,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AA53034-562E-444A-A174-EDCAB48FAF98}" name="Table14" displayName="Table14" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AA53034-562E-444A-A174-EDCAB48FAF98}" name="Table14" displayName="Table14" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:H1048576" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story #"/>
@@ -883,7 +894,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2BB48A9-B7C9-4465-A694-A1A60DB862A5}" name="Table13" displayName="Table13" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2BB48A9-B7C9-4465-A694-A1A60DB862A5}" name="Table13" displayName="Table13" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:G1048574" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story #"/>
@@ -899,10 +910,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53015D-1831-4CC7-AB65-5D7B71763781}" name="Table16" displayName="Table16" ref="A1:H37" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53015D-1831-4CC7-AB65-5D7B71763781}" name="Table16" displayName="Table16" ref="A1:H37" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:H37" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{60E2564F-7A0E-41C5-B5EF-E3B5C8DF36D3}" name="User Story " dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{60E2564F-7A0E-41C5-B5EF-E3B5C8DF36D3}" name="User Story " dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{BE915640-2681-4807-B9F9-EDDB87C59847}" name="Issue #"/>
     <tableColumn id="2" xr3:uid="{D190346C-2729-493C-BBAD-E061FA84D96B}" name="Task#"/>
     <tableColumn id="3" xr3:uid="{ED69C779-D47B-45D0-9B70-47CCE998BEA4}" name="Task assigned to"/>
@@ -916,7 +927,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E492D9C-8291-4D1A-B15F-F7CBDF216488}" name="Table15" displayName="Table15" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E492D9C-8291-4D1A-B15F-F7CBDF216488}" name="Table15" displayName="Table15" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:G1048574" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story #"/>
@@ -932,12 +943,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE1F1E48-758A-4606-B3B6-7A9876FFA9A6}" name="Table17" displayName="Table17" ref="A1:H37" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE1F1E48-758A-4606-B3B6-7A9876FFA9A6}" name="Table17" displayName="Table17" ref="A1:H37" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:H37" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7A20E7DE-AD4A-4D31-B30A-87F953C850B5}" name="User Story " dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{7A20E7DE-AD4A-4D31-B30A-87F953C850B5}" name="User Story " dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{CE04B1C4-291F-469E-8EDA-4B2E50F1E047}" name="Issue #"/>
-    <tableColumn id="2" xr3:uid="{BFE63EB1-FE70-4D90-96B2-63F2704505A1}" name="Task#" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{BFE63EB1-FE70-4D90-96B2-63F2704505A1}" name="Task#" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{8EA413FE-D781-49A6-82E4-A822FAC4AFF5}" name="Task assigned to"/>
     <tableColumn id="4" xr3:uid="{62470DFE-0C6D-4AE3-8552-7F81C0E56895}" name="Estimated Effort"/>
     <tableColumn id="5" xr3:uid="{667E60DB-E809-4D96-9D39-512072F7B841}" name="Actual Effort"/>
@@ -949,24 +960,24 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EC8F8F18-C67A-440D-98F3-5233B12B9399}" name="Table179" displayName="Table179" ref="A1:H37" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:H37" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{505BF37E-5559-4660-A5DC-6C45410B793D}" name="Table110" displayName="Table110" ref="A1:H32" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:H32" xr:uid="{505BF37E-5559-4660-A5DC-6C45410B793D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3BD4994F-C015-4524-B884-B65C1F8340A1}" name="User Story " dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{C0A07963-9078-42D9-8A76-F98DF20B83E3}" name="Issue #"/>
-    <tableColumn id="2" xr3:uid="{EFCCC7A8-8321-48D2-B098-6D9ABA30A577}" name="Task#" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{27498A06-FEA1-4AB6-B66A-7A08E4F696CF}" name="Task assigned to"/>
-    <tableColumn id="4" xr3:uid="{4230F616-7593-43DE-BC1C-8BA5ED0C2CB2}" name="Estimated Effort" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{69901A89-5785-4BFE-A01A-A3860137F9E4}" name="Actual Effort"/>
-    <tableColumn id="6" xr3:uid="{BEFDE914-5CF7-4505-B133-97360564A7E5}" name="Done (y/n)"/>
-    <tableColumn id="7" xr3:uid="{A0404802-C130-469A-A5AD-B2363DEFBE47}" name="Notes"/>
+    <tableColumn id="1" xr3:uid="{704C9CD8-3BF6-4B0E-BACA-F1309EDDA625}" name="User Story " dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{7D3DC4A2-D824-4AC6-B28B-E4B004072D06}" name="Issue #"/>
+    <tableColumn id="2" xr3:uid="{AD281654-9076-434C-B1FB-A950E5CDB066}" name="Task#"/>
+    <tableColumn id="3" xr3:uid="{4C2437AB-C242-4458-A59B-845AFA74A52E}" name="Task assigned to"/>
+    <tableColumn id="4" xr3:uid="{666313C8-518C-4B0C-82B0-3E551BBF3D5E}" name="Estimated Effort"/>
+    <tableColumn id="5" xr3:uid="{937BA98D-259D-4323-9992-B43CF96C0BB5}" name="Actual Effort"/>
+    <tableColumn id="6" xr3:uid="{4316299C-D110-46C1-950A-B84976815615}" name="Done (y/n)"/>
+    <tableColumn id="7" xr3:uid="{5F935EC2-37D0-41D9-B537-7134167896C3}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1264,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA45181-374E-4F18-A322-7A27A61D7E83}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3186,7 +3197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC608E94-FFE2-486E-A28F-5ACAAA8D4039}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -3908,20 +3919,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A6C4CF-DE87-4275-B695-18198795793D}">
-  <dimension ref="A1:J39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02015C5-B4F3-4064-A2E7-8C1E75BE1AE8}">
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="47" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="35.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
@@ -3935,13 +3946,13 @@
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -3956,32 +3967,22 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="56">
+        <v>44811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="8">
         <v>0</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="8">
-        <v>2</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" t="s">
         <v>10</v>
@@ -3997,9 +3998,9 @@
       <c r="B3" s="17">
         <v>0</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="59"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="3"/>
@@ -4017,9 +4018,9 @@
       <c r="B4" s="33">
         <v>0</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="33"/>
-      <c r="E4" s="60"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
       <c r="H4" s="36"/>
@@ -4031,9 +4032,9 @@
       <c r="B5" s="38">
         <v>0</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="38"/>
-      <c r="E5" s="61"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
       <c r="H5" s="39"/>
@@ -4045,28 +4046,12 @@
       <c r="B6" s="14">
         <v>3</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="51">
-        <v>2.5</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="52"/>
-      <c r="I6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" t="s">
-        <v>108</v>
-      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
@@ -4075,627 +4060,408 @@
       <c r="B7" s="21">
         <v>9</v>
       </c>
-      <c r="C7" s="53">
-        <v>3.4</v>
-      </c>
-      <c r="D7" s="54" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="54">
-        <v>3</v>
-      </c>
-      <c r="G7" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="55"/>
-      <c r="J7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="17" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="21">
+        <v>10</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="16">
+        <v>2</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="21">
+        <v>4</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="14">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="14">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="19">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="21">
+        <v>16</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="21">
+        <v>19</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16">
-        <v>1</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="17">
-        <v>3</v>
-      </c>
-      <c r="G9" s="17" t="s">
+      <c r="H16" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="21">
+        <v>20</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="21">
-        <v>10</v>
-      </c>
-      <c r="C10" s="44">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="22">
-        <v>6</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="16">
-        <v>2</v>
-      </c>
-      <c r="C11" s="41">
-        <v>4</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="17">
-        <v>4</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="56"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16">
-        <v>2</v>
-      </c>
-      <c r="C12" s="41">
-        <v>3</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="17">
-        <v>2</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="14">
-        <v>4</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="8">
-        <v>3</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="21">
         <v>21</v>
       </c>
-      <c r="B14" s="14">
-        <v>8</v>
-      </c>
-      <c r="C14" s="45">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="8">
-        <v>1</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="52"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19">
-        <v>8</v>
-      </c>
-      <c r="C15" s="46">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="5">
-        <v>3</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="21">
+        <v>14</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="21">
         <v>22</v>
       </c>
-      <c r="B16" s="14">
-        <v>7</v>
-      </c>
-      <c r="C16" s="45">
-        <v>1.2</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="8">
-        <v>6</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="52"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16">
-        <v>7</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="17">
-        <v>5</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19">
-        <v>7</v>
-      </c>
-      <c r="C18" s="46">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="5">
-        <v>2</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="19">
-        <v>15</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="21">
-        <v>16</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="62"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
-        <v>25</v>
+    <row r="21" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="29" t="s">
+        <v>76</v>
       </c>
       <c r="B21" s="21">
-        <v>19</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="62"/>
+        <v>17</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28" t="s">
-        <v>75</v>
+    <row r="22" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="27" t="s">
+        <v>29</v>
       </c>
       <c r="B22" s="21">
-        <v>20</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="62"/>
+        <v>18</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B23" s="21">
-        <v>21</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="62"/>
+        <v>23</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
       <c r="H23" s="23"/>
     </row>
-    <row r="24" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B24" s="21">
-        <v>14</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="62"/>
+        <v>24</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="27" t="s">
-        <v>28</v>
+    <row r="25" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="B25" s="21">
-        <v>22</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="62"/>
+        <v>30</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="29" t="s">
-        <v>76</v>
+    <row r="26" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="B26" s="21">
-        <v>17</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="62"/>
+        <v>31</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="27" t="s">
-        <v>29</v>
+    <row r="27" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="30" t="s">
+        <v>34</v>
       </c>
       <c r="B27" s="21">
-        <v>18</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="62"/>
+        <v>32</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
       <c r="H27" s="23"/>
     </row>
-    <row r="28" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="27" t="s">
-        <v>30</v>
+    <row r="28" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="B28" s="21">
-        <v>23</v>
-      </c>
-      <c r="C28" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="62"/>
+        <v>25</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="27" t="s">
-        <v>31</v>
+      <c r="A29" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="B29" s="21">
-        <v>24</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="62"/>
+        <v>26</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="23"/>
     </row>
     <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="30" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B30" s="21">
-        <v>30</v>
-      </c>
-      <c r="C30" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="62"/>
+        <v>27</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="23"/>
     </row>
-    <row r="31" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="30" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B31" s="21">
-        <v>31</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="62"/>
+        <v>28</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
     </row>
     <row r="32" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="30" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B32" s="21">
-        <v>32</v>
-      </c>
-      <c r="C32" s="46" t="s">
-        <v>109</v>
+        <v>29</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>108</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="62"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="H32" s="23"/>
     </row>
-    <row r="33" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="21">
-        <v>25</v>
-      </c>
-      <c r="C33" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="62"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="23"/>
-    </row>
-    <row r="34" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="21">
-        <v>26</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="62"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="23"/>
-    </row>
-    <row r="35" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="21">
-        <v>27</v>
-      </c>
-      <c r="C35" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="62"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="23"/>
-    </row>
-    <row r="36" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="21">
-        <v>28</v>
-      </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="23"/>
-    </row>
-    <row r="37" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="21">
-        <v>29</v>
-      </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="23"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="26"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add sprint info for Gijs
</commit_message>
<xml_diff>
--- a/doc/sprints.xlsx
+++ b/doc/sprints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauli\Documents\TU\repositories\SEM\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gvand\IdeaProjects\sem-repo-17a\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827ABC23-4561-491F-986F-C731C398454B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98428D8A-3BC3-4FAA-8509-C36624168ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30105" yWindow="660" windowWidth="20250" windowHeight="11280" tabRatio="671" activeTab="3" xr2:uid="{58667ADA-671B-4355-9B89-7418DDCFDFF4}"/>
+    <workbookView xWindow="17760" yWindow="1725" windowWidth="21600" windowHeight="11385" tabRatio="671" firstSheet="4" activeTab="5" xr2:uid="{58667ADA-671B-4355-9B89-7418DDCFDFF4}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="128">
   <si>
     <t>User Story #</t>
   </si>
@@ -390,6 +390,39 @@
   </si>
   <si>
     <t>ended up being needed in different format</t>
+  </si>
+  <si>
+    <t>Gijs</t>
+  </si>
+  <si>
+    <t>6-8 hours</t>
+  </si>
+  <si>
+    <t>14 hours</t>
+  </si>
+  <si>
+    <t>See sprint retrospectives.</t>
+  </si>
+  <si>
+    <t>Pauline, Gijs</t>
+  </si>
+  <si>
+    <t>P:1, G:2</t>
+  </si>
+  <si>
+    <t>P:1 , G:3</t>
+  </si>
+  <si>
+    <t>2-3 hours</t>
+  </si>
+  <si>
+    <t>P: 1.2 G: rest</t>
+  </si>
+  <si>
+    <t>P:1, G:2-3</t>
+  </si>
+  <si>
+    <t>P:1 , G:3.5</t>
   </si>
 </sst>
 </file>
@@ -591,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -683,9 +716,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -943,7 +977,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1245,20 +1279,20 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -1287,7 +1321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>44</v>
       </c>
@@ -1307,7 +1341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>49</v>
       </c>
@@ -1327,7 +1361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>80</v>
       </c>
@@ -1341,7 +1375,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="36"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>81</v>
       </c>
@@ -1355,7 +1389,7 @@
       <c r="G5" s="38"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +1403,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +1417,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="23"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>17</v>
       </c>
@@ -1397,7 +1431,7 @@
       <c r="G8" s="17"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>18</v>
       </c>
@@ -1411,7 +1445,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
@@ -1425,7 +1459,7 @@
       <c r="G10" s="17"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>20</v>
       </c>
@@ -1439,7 +1473,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>21</v>
       </c>
@@ -1453,7 +1487,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>22</v>
       </c>
@@ -1467,7 +1501,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>23</v>
       </c>
@@ -1481,7 +1515,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>24</v>
       </c>
@@ -1495,7 +1529,7 @@
       <c r="G15" s="22"/>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="1:10" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>25</v>
       </c>
@@ -1509,7 +1543,7 @@
       <c r="G16" s="22"/>
       <c r="H16" s="23"/>
     </row>
-    <row r="17" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>70</v>
       </c>
@@ -1523,7 +1557,7 @@
       <c r="G17" s="22"/>
       <c r="H17" s="23"/>
     </row>
-    <row r="18" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>26</v>
       </c>
@@ -1537,7 +1571,7 @@
       <c r="G18" s="22"/>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>27</v>
       </c>
@@ -1551,7 +1585,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>28</v>
       </c>
@@ -1565,7 +1599,7 @@
       <c r="G20" s="22"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>71</v>
       </c>
@@ -1579,7 +1613,7 @@
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>29</v>
       </c>
@@ -1593,7 +1627,7 @@
       <c r="G22" s="22"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>30</v>
       </c>
@@ -1607,7 +1641,7 @@
       <c r="G23" s="22"/>
       <c r="H23" s="23"/>
     </row>
-    <row r="24" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>31</v>
       </c>
@@ -1621,7 +1655,7 @@
       <c r="G24" s="22"/>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>32</v>
       </c>
@@ -1635,7 +1669,7 @@
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
         <v>33</v>
       </c>
@@ -1649,7 +1683,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
         <v>34</v>
       </c>
@@ -1663,7 +1697,7 @@
       <c r="G27" s="22"/>
       <c r="H27" s="23"/>
     </row>
-    <row r="28" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
         <v>35</v>
       </c>
@@ -1677,7 +1711,7 @@
       <c r="G28" s="22"/>
       <c r="H28" s="23"/>
     </row>
-    <row r="29" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
         <v>36</v>
       </c>
@@ -1691,7 +1725,7 @@
       <c r="G29" s="22"/>
       <c r="H29" s="23"/>
     </row>
-    <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
         <v>37</v>
       </c>
@@ -1705,7 +1739,7 @@
       <c r="G30" s="22"/>
       <c r="H30" s="23"/>
     </row>
-    <row r="31" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>38</v>
       </c>
@@ -1719,7 +1753,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
     </row>
-    <row r="32" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>39</v>
       </c>
@@ -1733,11 +1767,11 @@
       <c r="G32" s="22"/>
       <c r="H32" s="23"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="26"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="26"/>
     </row>
@@ -1758,18 +1792,18 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1"/>
-    <col min="3" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>63</v>
       </c>
@@ -1823,7 +1857,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>61</v>
@@ -1839,7 +1873,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="5" t="s">
         <v>59</v>
@@ -1859,7 +1893,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>49</v>
       </c>
@@ -1887,7 +1921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="5" t="s">
         <v>56</v>
@@ -1915,10 +1949,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="I8" t="s">
         <v>51</v>
@@ -1927,79 +1961,79 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
   </sheetData>
@@ -2019,18 +2053,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" customWidth="1"/>
-    <col min="3" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2059,7 +2093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>49</v>
       </c>
@@ -2088,7 +2122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="5" t="s">
         <v>46</v>
@@ -2113,7 +2147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>44</v>
       </c>
@@ -2130,7 +2164,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="17" t="s">
         <v>42</v>
@@ -2145,7 +2179,7 @@
       <c r="F5" s="17"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="5" t="s">
         <v>41</v>
@@ -2160,79 +2194,79 @@
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
   </sheetData>
@@ -2248,24 +2282,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D43D420-8132-4A0A-B840-CA93FDE81F26}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="81.21875" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="81.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -2297,7 +2331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>44</v>
       </c>
@@ -2327,7 +2361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="33">
         <v>0</v>
@@ -2355,7 +2389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="35"/>
       <c r="B4" s="33"/>
       <c r="C4" s="17" t="s">
@@ -2375,7 +2409,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="33">
         <v>0</v>
@@ -2397,7 +2431,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -2417,7 +2451,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>49</v>
       </c>
@@ -2447,7 +2481,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
       <c r="B8" s="33">
         <v>0</v>
@@ -2469,7 +2503,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="35"/>
       <c r="B9" s="33"/>
       <c r="C9" s="17" t="s">
@@ -2491,7 +2525,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>80</v>
       </c>
@@ -2505,7 +2539,7 @@
       <c r="G10" s="33"/>
       <c r="H10" s="36"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>81</v>
       </c>
@@ -2519,7 +2553,7 @@
       <c r="G11" s="38"/>
       <c r="H11" s="39"/>
     </row>
-    <row r="12" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
@@ -2533,7 +2567,7 @@
       <c r="G12" s="22"/>
       <c r="H12" s="23"/>
     </row>
-    <row r="13" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>16</v>
       </c>
@@ -2547,7 +2581,7 @@
       <c r="G13" s="22"/>
       <c r="H13" s="23"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>17</v>
       </c>
@@ -2561,7 +2595,7 @@
       <c r="G14" s="17"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>18</v>
       </c>
@@ -2575,7 +2609,7 @@
       <c r="G15" s="22"/>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
@@ -2589,7 +2623,7 @@
       <c r="G16" s="17"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>20</v>
       </c>
@@ -2603,7 +2637,7 @@
       <c r="G17" s="22"/>
       <c r="H17" s="23"/>
     </row>
-    <row r="18" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>21</v>
       </c>
@@ -2617,7 +2651,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>22</v>
       </c>
@@ -2631,7 +2665,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>23</v>
       </c>
@@ -2645,7 +2679,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>24</v>
       </c>
@@ -2659,7 +2693,7 @@
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>25</v>
       </c>
@@ -2673,7 +2707,7 @@
       <c r="G22" s="22"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
         <v>70</v>
       </c>
@@ -2687,7 +2721,7 @@
       <c r="G23" s="22"/>
       <c r="H23" s="23"/>
     </row>
-    <row r="24" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>26</v>
       </c>
@@ -2701,7 +2735,7 @@
       <c r="G24" s="22"/>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>27</v>
       </c>
@@ -2715,7 +2749,7 @@
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>28</v>
       </c>
@@ -2729,7 +2763,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>71</v>
       </c>
@@ -2743,7 +2777,7 @@
       <c r="G27" s="22"/>
       <c r="H27" s="23"/>
     </row>
-    <row r="28" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>29</v>
       </c>
@@ -2757,7 +2791,7 @@
       <c r="G28" s="22"/>
       <c r="H28" s="23"/>
     </row>
-    <row r="29" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>30</v>
       </c>
@@ -2771,7 +2805,7 @@
       <c r="G29" s="22"/>
       <c r="H29" s="23"/>
     </row>
-    <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>31</v>
       </c>
@@ -2785,7 +2819,7 @@
       <c r="G30" s="22"/>
       <c r="H30" s="23"/>
     </row>
-    <row r="31" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>32</v>
       </c>
@@ -2799,7 +2833,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
     </row>
-    <row r="32" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>33</v>
       </c>
@@ -2813,7 +2847,7 @@
       <c r="G32" s="22"/>
       <c r="H32" s="23"/>
     </row>
-    <row r="33" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
         <v>34</v>
       </c>
@@ -2827,7 +2861,7 @@
       <c r="G33" s="22"/>
       <c r="H33" s="23"/>
     </row>
-    <row r="34" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
         <v>35</v>
       </c>
@@ -2841,7 +2875,7 @@
       <c r="G34" s="22"/>
       <c r="H34" s="23"/>
     </row>
-    <row r="35" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
         <v>36</v>
       </c>
@@ -2855,7 +2889,7 @@
       <c r="G35" s="22"/>
       <c r="H35" s="23"/>
     </row>
-    <row r="36" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
         <v>37</v>
       </c>
@@ -2869,7 +2903,7 @@
       <c r="G36" s="22"/>
       <c r="H36" s="23"/>
     </row>
-    <row r="37" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>38</v>
       </c>
@@ -2883,7 +2917,7 @@
       <c r="G37" s="22"/>
       <c r="H37" s="23"/>
     </row>
-    <row r="38" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>39</v>
       </c>
@@ -2897,11 +2931,11 @@
       <c r="G38" s="22"/>
       <c r="H38" s="23"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
       <c r="B39" s="26"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="26"/>
     </row>
@@ -2919,23 +2953,23 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="47" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -2967,7 +3001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>44</v>
       </c>
@@ -2997,7 +3031,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>44</v>
       </c>
@@ -3027,7 +3061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>49</v>
       </c>
@@ -3041,7 +3075,7 @@
       <c r="G4" s="17"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>80</v>
       </c>
@@ -3055,7 +3089,7 @@
       <c r="G5" s="33"/>
       <c r="H5" s="36"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>81</v>
       </c>
@@ -3075,7 +3109,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -3102,7 +3136,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -3126,7 +3160,7 @@
       </c>
       <c r="H8" s="55"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
@@ -3150,7 +3184,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="16">
         <v>1</v>
@@ -3172,7 +3206,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
@@ -3196,7 +3230,7 @@
       </c>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
@@ -3220,7 +3254,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
       <c r="B13" s="16">
         <v>2</v>
@@ -3242,7 +3276,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>20</v>
       </c>
@@ -3266,7 +3300,7 @@
       </c>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>21</v>
       </c>
@@ -3290,7 +3324,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="19">
         <v>8</v>
@@ -3312,7 +3346,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
@@ -3336,7 +3370,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="16">
         <v>7</v>
@@ -3358,7 +3392,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="19">
         <v>7</v>
@@ -3380,7 +3414,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>23</v>
       </c>
@@ -3394,7 +3428,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>24</v>
       </c>
@@ -3408,7 +3442,7 @@
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>25</v>
       </c>
@@ -3422,7 +3456,7 @@
       <c r="G22" s="22"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
         <v>70</v>
       </c>
@@ -3436,7 +3470,7 @@
       <c r="G23" s="22"/>
       <c r="H23" s="23"/>
     </row>
-    <row r="24" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>26</v>
       </c>
@@ -3450,7 +3484,7 @@
       <c r="G24" s="22"/>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>27</v>
       </c>
@@ -3464,7 +3498,7 @@
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>28</v>
       </c>
@@ -3478,7 +3512,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>71</v>
       </c>
@@ -3492,7 +3526,7 @@
       <c r="G27" s="22"/>
       <c r="H27" s="23"/>
     </row>
-    <row r="28" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>29</v>
       </c>
@@ -3506,7 +3540,7 @@
       <c r="G28" s="22"/>
       <c r="H28" s="23"/>
     </row>
-    <row r="29" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>30</v>
       </c>
@@ -3520,7 +3554,7 @@
       <c r="G29" s="22"/>
       <c r="H29" s="23"/>
     </row>
-    <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>31</v>
       </c>
@@ -3534,7 +3568,7 @@
       <c r="G30" s="22"/>
       <c r="H30" s="23"/>
     </row>
-    <row r="31" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>32</v>
       </c>
@@ -3548,7 +3582,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
     </row>
-    <row r="32" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>33</v>
       </c>
@@ -3562,7 +3596,7 @@
       <c r="G32" s="22"/>
       <c r="H32" s="23"/>
     </row>
-    <row r="33" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
         <v>34</v>
       </c>
@@ -3576,7 +3610,7 @@
       <c r="G33" s="22"/>
       <c r="H33" s="23"/>
     </row>
-    <row r="34" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
         <v>35</v>
       </c>
@@ -3590,7 +3624,7 @@
       <c r="G34" s="22"/>
       <c r="H34" s="23"/>
     </row>
-    <row r="35" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
         <v>36</v>
       </c>
@@ -3604,7 +3638,7 @@
       <c r="G35" s="22"/>
       <c r="H35" s="23"/>
     </row>
-    <row r="36" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
         <v>37</v>
       </c>
@@ -3618,7 +3652,7 @@
       <c r="G36" s="22"/>
       <c r="H36" s="23"/>
     </row>
-    <row r="37" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>38</v>
       </c>
@@ -3632,7 +3666,7 @@
       <c r="G37" s="22"/>
       <c r="H37" s="23"/>
     </row>
-    <row r="38" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>39</v>
       </c>
@@ -3646,11 +3680,11 @@
       <c r="G38" s="22"/>
       <c r="H38" s="23"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
       <c r="B39" s="26"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="26"/>
     </row>
@@ -3667,24 +3701,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02015C5-B4F3-4064-A2E7-8C1E75BE1AE8}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -3716,7 +3750,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>44</v>
       </c>
@@ -3736,7 +3770,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>49</v>
       </c>
@@ -3756,7 +3790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>80</v>
       </c>
@@ -3770,7 +3804,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="36"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>81</v>
       </c>
@@ -3784,7 +3818,7 @@
       <c r="G5" s="38"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
@@ -3798,7 +3832,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>16</v>
       </c>
@@ -3812,7 +3846,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="23"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>17</v>
       </c>
@@ -3826,7 +3860,7 @@
       <c r="G8" s="17"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>18</v>
       </c>
@@ -3840,7 +3874,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
@@ -3848,13 +3882,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="17">
+        <v>4</v>
+      </c>
       <c r="G10" s="17"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>20</v>
       </c>
@@ -3878,7 +3918,7 @@
       </c>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>21</v>
       </c>
@@ -3889,42 +3929,44 @@
         <v>110</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8"/>
+        <v>121</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="14">
         <v>7</v>
       </c>
-      <c r="C13" s="8">
-        <v>1.2</v>
+      <c r="C13" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>23</v>
       </c>
@@ -3948,7 +3990,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>24</v>
       </c>
@@ -3972,7 +4014,7 @@
       </c>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="1:10" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>25</v>
       </c>
@@ -3998,7 +4040,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>70</v>
       </c>
@@ -4022,7 +4064,7 @@
       </c>
       <c r="H17" s="23"/>
     </row>
-    <row r="18" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>26</v>
       </c>
@@ -4048,7 +4090,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>27</v>
       </c>
@@ -4072,21 +4114,33 @@
       </c>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="21">
         <v>22</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
-    </row>
-    <row r="21" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>71</v>
       </c>
@@ -4100,7 +4154,7 @@
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>29</v>
       </c>
@@ -4114,7 +4168,7 @@
       <c r="G22" s="22"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>30</v>
       </c>
@@ -4138,21 +4192,31 @@
       </c>
       <c r="H23" s="23"/>
     </row>
-    <row r="24" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="21">
         <v>24</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
+      <c r="C24" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="22">
+        <v>2</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>32</v>
       </c>
@@ -4166,7 +4230,7 @@
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
         <v>33</v>
       </c>
@@ -4180,7 +4244,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
         <v>34</v>
       </c>
@@ -4194,7 +4258,7 @@
       <c r="G27" s="22"/>
       <c r="H27" s="23"/>
     </row>
-    <row r="28" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
         <v>35</v>
       </c>
@@ -4208,7 +4272,7 @@
       <c r="G28" s="22"/>
       <c r="H28" s="23"/>
     </row>
-    <row r="29" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
         <v>36</v>
       </c>
@@ -4232,7 +4296,7 @@
       </c>
       <c r="H29" s="23"/>
     </row>
-    <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
         <v>37</v>
       </c>
@@ -4256,7 +4320,7 @@
       </c>
       <c r="H30" s="23"/>
     </row>
-    <row r="31" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>38</v>
       </c>
@@ -4270,7 +4334,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
     </row>
-    <row r="32" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>39</v>
       </c>
@@ -4294,11 +4358,11 @@
       </c>
       <c r="H32" s="23"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="26"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="26"/>
     </row>

</xml_diff>